<commit_message>
Added automatic coloring to plots
</commit_message>
<xml_diff>
--- a/manual_analysis/chi_squared.xlsx
+++ b/manual_analysis/chi_squared.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ualbertaca-my.sharepoint.com/personal/hqiu1_ualberta_ca/Documents/Coding/TBI Clustering/analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ualbertaca-my.sharepoint.com/personal/hqiu1_ualberta_ca/Documents/Coding/TBI_Clustering/manual_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="162" documentId="8_{8BD920B0-DD1B-4496-92DA-EF1972C56E34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0021A89-779F-40BE-BDC6-0CAA9788B0BA}"/>
+  <xr:revisionPtr revIDLastSave="186" documentId="8_{8BD920B0-DD1B-4496-92DA-EF1972C56E34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39E46683-7F6F-4072-A9B9-78290391C028}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="10690" windowWidth="19420" windowHeight="10420" xr2:uid="{C216D06F-6D43-461A-ADEC-166DBF3A6BBE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="22">
   <si>
     <t>Alive</t>
   </si>
@@ -84,6 +84,24 @@
   </si>
   <si>
     <t>Endotype 8</t>
+  </si>
+  <si>
+    <t>For SPSS</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Endotype</t>
+  </si>
+  <si>
+    <t>Need to weight by frequency first</t>
+  </si>
+  <si>
+    <t>Notes: Weight by frequency (under data→weight), crosstabs, select options for Chi square under "tests", select column comparisons with bonferroni adjustment under "cells", put endotype as columns and status as row</t>
   </si>
 </sst>
 </file>
@@ -2621,16 +2639,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>102870</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>288290</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>36830</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>407670</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>593090</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>36830</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2993,8 +3011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60A6EB47-E76C-4062-97B6-B94F79BF9924}">
   <dimension ref="A1:S36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
-      <selection activeCell="U25" sqref="U25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3745,10 +3763,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FF329A4-1189-4B50-A024-424B59A1F7D9}">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3758,10 +3776,10 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -3875,7 +3893,46 @@
         <v>0.55533596837944665</v>
       </c>
     </row>
-    <row r="17" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>441</v>
+      </c>
       <c r="E17">
         <v>47</v>
       </c>
@@ -3883,7 +3940,16 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>147</v>
+      </c>
       <c r="E18">
         <v>441</v>
       </c>
@@ -3891,7 +3957,16 @@
         <v>428</v>
       </c>
     </row>
-    <row r="19" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>33</v>
+      </c>
       <c r="E19">
         <v>147</v>
       </c>
@@ -3899,7 +3974,16 @@
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>121</v>
+      </c>
       <c r="E20">
         <v>33</v>
       </c>
@@ -3907,7 +3991,16 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>320</v>
+      </c>
       <c r="E21">
         <v>121</v>
       </c>
@@ -3915,7 +4008,16 @@
         <v>115</v>
       </c>
     </row>
-    <row r="22" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>76</v>
+      </c>
       <c r="E22">
         <v>320</v>
       </c>
@@ -3923,7 +4025,16 @@
         <v>948</v>
       </c>
     </row>
-    <row r="23" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>54</v>
+      </c>
       <c r="E23">
         <v>76</v>
       </c>
@@ -3931,16 +4042,108 @@
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>11</v>
+      </c>
       <c r="E24">
         <v>54</v>
       </c>
       <c r="F24">
         <v>112</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>